<commit_message>
bijgewerkt voor tcs versie
</commit_message>
<xml_diff>
--- a/uml/IMKL2.x/IMKL-UML-XSD-Objectcatalogus-changelog.xlsx
+++ b/uml/IMKL2.x/IMKL-UML-XSD-Objectcatalogus-changelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-dev\uml\IMKL2.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A557C3B4-C2AA-42BB-BD1F-706D8E19B78C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55176142-236B-432D-81ED-8A46B8B73236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
+    <workbookView xWindow="630" yWindow="1485" windowWidth="37095" windowHeight="13935" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="119">
   <si>
     <t>Datum</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t>nvt</t>
+  </si>
+  <si>
+    <t>nietaangepast</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,12 +524,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +542,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -593,9 +590,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -932,7 +926,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1482,31 +1476,31 @@
       </c>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21">
+    <row r="21" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20">
         <v>43943</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" s="22">
+      <c r="H21" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="21">
         <v>193</v>
       </c>
-      <c r="J21" s="21"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
@@ -1560,7 +1554,7 @@
       </c>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>43944</v>
       </c>
@@ -1579,7 +1573,7 @@
       <c r="H24" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="18"/>
       <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -2061,7 +2055,9 @@
       <c r="F44" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G44" s="18"/>
+      <c r="G44" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="H44" s="6" t="s">
         <v>114</v>
       </c>
@@ -2081,7 +2077,9 @@
       <c r="F45" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G45" s="18"/>
+      <c r="G45" s="12" t="s">
+        <v>118</v>
+      </c>
       <c r="H45" s="6" t="s">
         <v>114</v>
       </c>
@@ -2309,7 +2307,9 @@
       <c r="F54" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G54" s="18"/>
+      <c r="G54" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="H54" s="6" t="s">
         <v>114</v>
       </c>
@@ -3987,6 +3987,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003ADD3040E3157B4E913BCA65F34844D7" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c1765059aa1475931adc12138fdcfd8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aafb19fa-82be-411d-a6df-c75e9235a4ea" xmlns:ns3="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42d79c55539af1f9f274032ce6041302" ns2:_="" ns3:_="">
     <xsd:import namespace="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
@@ -4189,15 +4198,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
   <ds:schemaRefs>
@@ -4208,6 +4208,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0C9FDDB-2830-4DD6-A847-D844746B12F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4224,12 +4232,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>